<commit_message>
Adding IMU and update board outline to 39mm square
</commit_message>
<xml_diff>
--- a/Gerber/CPL_JLCSMT.xlsx
+++ b/Gerber/CPL_JLCSMT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\will1\Dropbox\KiCad\IMX283_MIPI_Camera_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE46FFF-E61C-4C3B-A7BA-FB8F13C5A35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B251DE-AFC6-48E5-B327-B72D7A2CE684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14483" yWindow="1868" windowWidth="22335" windowHeight="17025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4777" yWindow="4523" windowWidth="22816" windowHeight="16792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="83">
   <si>
     <t>Designator</t>
   </si>
@@ -49,202 +49,226 @@
     <t>C3</t>
   </si>
   <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>C16</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>C20</t>
+  </si>
+  <si>
+    <t>C21</t>
+  </si>
+  <si>
+    <t>C22</t>
+  </si>
+  <si>
+    <t>C23</t>
+  </si>
+  <si>
+    <t>C24</t>
+  </si>
+  <si>
+    <t>C25</t>
+  </si>
+  <si>
+    <t>C26</t>
+  </si>
+  <si>
+    <t>C27</t>
+  </si>
+  <si>
+    <t>C28</t>
+  </si>
+  <si>
+    <t>C29</t>
+  </si>
+  <si>
+    <t>C30</t>
+  </si>
+  <si>
+    <t>C31</t>
+  </si>
+  <si>
+    <t>C32</t>
+  </si>
+  <si>
+    <t>C33</t>
+  </si>
+  <si>
+    <t>C34</t>
+  </si>
+  <si>
+    <t>C35</t>
+  </si>
+  <si>
+    <t>C36</t>
+  </si>
+  <si>
+    <t>C37</t>
+  </si>
+  <si>
+    <t>C38</t>
+  </si>
+  <si>
+    <t>FB1</t>
+  </si>
+  <si>
+    <t>FB2</t>
+  </si>
+  <si>
+    <t>FB3</t>
+  </si>
+  <si>
+    <t>FL1</t>
+  </si>
+  <si>
+    <t>FL2</t>
+  </si>
+  <si>
+    <t>FL3</t>
+  </si>
+  <si>
+    <t>FL4</t>
+  </si>
+  <si>
+    <t>FL5</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>C39</t>
+  </si>
+  <si>
+    <t>C40</t>
+  </si>
+  <si>
+    <t>C41</t>
+  </si>
+  <si>
+    <t>FB4</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>JPR1</t>
+  </si>
+  <si>
+    <t>JPR2</t>
+  </si>
+  <si>
+    <t>C42</t>
+  </si>
+  <si>
+    <t>C43</t>
+  </si>
+  <si>
+    <t>C44</t>
+  </si>
+  <si>
     <t>R2</t>
   </si>
   <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>C6</t>
-  </si>
-  <si>
-    <t>C7</t>
-  </si>
-  <si>
-    <t>C8</t>
-  </si>
-  <si>
-    <t>C9</t>
-  </si>
-  <si>
-    <t>C10</t>
-  </si>
-  <si>
-    <t>C11</t>
-  </si>
-  <si>
-    <t>C12</t>
-  </si>
-  <si>
-    <t>C13</t>
-  </si>
-  <si>
-    <t>C14</t>
-  </si>
-  <si>
-    <t>C15</t>
-  </si>
-  <si>
-    <t>C16</t>
-  </si>
-  <si>
-    <t>C17</t>
-  </si>
-  <si>
-    <t>C18</t>
-  </si>
-  <si>
-    <t>C19</t>
-  </si>
-  <si>
-    <t>C20</t>
-  </si>
-  <si>
-    <t>C21</t>
-  </si>
-  <si>
-    <t>C22</t>
-  </si>
-  <si>
-    <t>C23</t>
-  </si>
-  <si>
-    <t>C24</t>
-  </si>
-  <si>
-    <t>C25</t>
-  </si>
-  <si>
-    <t>C26</t>
-  </si>
-  <si>
-    <t>C27</t>
-  </si>
-  <si>
-    <t>C28</t>
-  </si>
-  <si>
-    <t>C29</t>
-  </si>
-  <si>
-    <t>C30</t>
-  </si>
-  <si>
-    <t>C31</t>
-  </si>
-  <si>
-    <t>C32</t>
-  </si>
-  <si>
-    <t>C33</t>
-  </si>
-  <si>
-    <t>C34</t>
-  </si>
-  <si>
-    <t>C35</t>
-  </si>
-  <si>
-    <t>C36</t>
-  </si>
-  <si>
-    <t>C37</t>
-  </si>
-  <si>
-    <t>C38</t>
-  </si>
-  <si>
-    <t>FB1</t>
-  </si>
-  <si>
-    <t>FB2</t>
-  </si>
-  <si>
-    <t>FB3</t>
-  </si>
-  <si>
-    <t>FL1</t>
-  </si>
-  <si>
-    <t>FL2</t>
-  </si>
-  <si>
-    <t>FL3</t>
-  </si>
-  <si>
-    <t>FL4</t>
-  </si>
-  <si>
-    <t>FL5</t>
-  </si>
-  <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>J2</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
     <t>R3</t>
   </si>
   <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>U6</t>
-  </si>
-  <si>
-    <t>C39</t>
-  </si>
-  <si>
-    <t>C40</t>
-  </si>
-  <si>
-    <t>C41</t>
-  </si>
-  <si>
-    <t>FB4</t>
-  </si>
-  <si>
-    <t>R9</t>
-  </si>
-  <si>
-    <t>U7</t>
-  </si>
-  <si>
-    <t>U8</t>
+    <t>U9</t>
   </si>
 </sst>
 </file>
@@ -593,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
@@ -630,10 +654,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>136.4</v>
+        <v>143.1</v>
       </c>
       <c r="C2" s="2">
-        <v>-96.9</v>
+        <v>-92.85</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -647,10 +671,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="2">
-        <v>146.4</v>
+        <v>153.6</v>
       </c>
       <c r="C3" s="2">
-        <v>-105.6</v>
+        <v>-101.7</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -664,10 +688,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="2">
-        <v>140.9</v>
+        <v>147.6</v>
       </c>
       <c r="C4" s="2">
-        <v>-97.02</v>
+        <v>-92.85</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
@@ -678,13 +702,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2">
-        <v>145.9</v>
+        <v>152.6</v>
       </c>
       <c r="C5" s="2">
-        <v>-97</v>
+        <v>-92.85</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
@@ -695,13 +719,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2">
-        <v>144.68</v>
+        <v>151.4</v>
       </c>
       <c r="C6" s="2">
-        <v>-100.8</v>
+        <v>-96.1</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>6</v>
@@ -712,13 +736,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2">
-        <v>143.9</v>
+        <v>150.6</v>
       </c>
       <c r="C7" s="2">
-        <v>-97</v>
+        <v>-92.85</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
@@ -729,13 +753,13 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2">
-        <v>145.9</v>
+        <v>152.6</v>
       </c>
       <c r="C8" s="2">
-        <v>-110.6</v>
+        <v>-106.35</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
@@ -746,13 +770,13 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2">
-        <v>144.6</v>
+        <v>151.35</v>
       </c>
       <c r="C9" s="2">
-        <v>-106.8</v>
+        <v>-102.6</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>6</v>
@@ -763,13 +787,13 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2">
-        <v>136.4</v>
+        <v>143.1</v>
       </c>
       <c r="C10" s="2">
-        <v>-110.7</v>
+        <v>-106.5</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>6</v>
@@ -780,13 +804,13 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2">
-        <v>142.4</v>
+        <v>149.1</v>
       </c>
       <c r="C11" s="2">
-        <v>-100.08</v>
+        <v>-95.88</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>6</v>
@@ -797,13 +821,13 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2">
-        <v>140.9</v>
+        <v>147.6</v>
       </c>
       <c r="C12" s="2">
-        <v>-110.6</v>
+        <v>-106.35</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>6</v>
@@ -814,13 +838,13 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="2">
-        <v>144.69999999999999</v>
+        <v>151.4</v>
       </c>
       <c r="C13" s="2">
-        <v>-101.8</v>
+        <v>-97.1</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>6</v>
@@ -831,13 +855,13 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2">
-        <v>132.68</v>
+        <v>139.38</v>
       </c>
       <c r="C14" s="2">
-        <v>-99.3</v>
+        <v>-95.1</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>6</v>
@@ -848,13 +872,13 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="2">
-        <v>143.9</v>
+        <v>150.6</v>
       </c>
       <c r="C15" s="2">
-        <v>-110.6</v>
+        <v>-106.35</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>6</v>
@@ -865,13 +889,13 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="2">
-        <v>144.6</v>
+        <v>151.35</v>
       </c>
       <c r="C16" s="2">
-        <v>-105.35</v>
+        <v>-101.1</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>6</v>
@@ -882,13 +906,13 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="2">
-        <v>132.69999999999999</v>
+        <v>139.15</v>
       </c>
       <c r="C17" s="2">
-        <v>-100.9</v>
+        <v>-96.6</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>6</v>
@@ -899,13 +923,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="2">
-        <v>145</v>
+        <v>151.69999999999999</v>
       </c>
       <c r="C18" s="2">
-        <v>-97</v>
+        <v>-92.85</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>6</v>
@@ -916,13 +940,13 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="2">
-        <v>131.80000000000001</v>
+        <v>138.55000000000001</v>
       </c>
       <c r="C19" s="2">
-        <v>-104.53749999999999</v>
+        <v>-100.33750000000001</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>6</v>
@@ -933,13 +957,13 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="2">
-        <v>144.9</v>
+        <v>151.6</v>
       </c>
       <c r="C20" s="2">
-        <v>-110.6</v>
+        <v>-106.35</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>6</v>
@@ -950,13 +974,13 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="2">
-        <v>132.69999999999999</v>
+        <v>139.35</v>
       </c>
       <c r="C21" s="2">
-        <v>-106.8</v>
+        <v>-102.6</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>6</v>
@@ -967,13 +991,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="2">
-        <v>146.4</v>
+        <v>153.6</v>
       </c>
       <c r="C22" s="2">
-        <v>-107.6</v>
+        <v>-103.55</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>6</v>
@@ -984,13 +1008,13 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" s="2">
-        <v>132.6</v>
+        <v>139.35</v>
       </c>
       <c r="C23" s="2">
-        <v>-108.3</v>
+        <v>-104.1</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>6</v>
@@ -1001,13 +1025,13 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="2">
-        <v>134.4</v>
+        <v>141.1</v>
       </c>
       <c r="C24" s="2">
-        <v>-96.337500000000006</v>
+        <v>-92.137500000000003</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>6</v>
@@ -1018,30 +1042,30 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="2">
-        <v>146.9</v>
+        <v>153.6</v>
       </c>
       <c r="C25" s="2">
-        <v>-109.1375</v>
+        <v>-106.35</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E25" s="2">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="2">
-        <v>150.52500000000001</v>
+        <v>157.32499999999999</v>
       </c>
       <c r="C26" s="2">
-        <v>-88.037499999999994</v>
+        <v>-83.8</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>6</v>
@@ -1052,13 +1076,13 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" s="2">
-        <v>132</v>
+        <v>138.75</v>
       </c>
       <c r="C27" s="2">
-        <v>-86.337500000000006</v>
+        <v>-83.8</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>6</v>
@@ -1069,13 +1093,13 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" s="2">
-        <v>134.9</v>
+        <v>141.6</v>
       </c>
       <c r="C28" s="2">
-        <v>-110.6</v>
+        <v>-106.35</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>6</v>
@@ -1086,13 +1110,13 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" s="2">
-        <v>135</v>
+        <v>141.69999999999999</v>
       </c>
       <c r="C29" s="2">
-        <v>-98.537499999999994</v>
+        <v>-94.337500000000006</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>6</v>
@@ -1103,13 +1127,13 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" s="2">
-        <v>134.58000000000001</v>
+        <v>141</v>
       </c>
       <c r="C30" s="2">
-        <v>-100.9</v>
+        <v>-96.6</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>6</v>
@@ -1120,13 +1144,13 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" s="2">
-        <v>136.4</v>
+        <v>143.1</v>
       </c>
       <c r="C31" s="2">
-        <v>-108.9</v>
+        <v>-104.7</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>6</v>
@@ -1137,13 +1161,13 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" s="2">
-        <v>134.1</v>
+        <v>140.85</v>
       </c>
       <c r="C32" s="2">
-        <v>-102.3</v>
+        <v>-98.1</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>6</v>
@@ -1154,13 +1178,13 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="2">
-        <v>133.4</v>
+        <v>140.15</v>
       </c>
       <c r="C33" s="2">
-        <v>-104.53749999999999</v>
+        <v>-100.33750000000001</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>6</v>
@@ -1171,30 +1195,30 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B34" s="2">
-        <v>150.625</v>
+        <v>159.85</v>
       </c>
       <c r="C34" s="2">
-        <v>-93.837500000000006</v>
+        <v>-87.375</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E34" s="2">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B35" s="2">
-        <v>132.07499999999999</v>
+        <v>138.69999999999999</v>
       </c>
       <c r="C35" s="2">
-        <v>-92.737499999999997</v>
+        <v>-89.8</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>6</v>
@@ -1205,13 +1229,13 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B36" s="2">
-        <v>143.9</v>
+        <v>150.6</v>
       </c>
       <c r="C36" s="2">
-        <v>-112.6875</v>
+        <v>-108.5</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>6</v>
@@ -1222,13 +1246,13 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B37" s="2">
-        <v>151</v>
+        <v>156.05000000000001</v>
       </c>
       <c r="C37" s="2">
-        <v>-95.037499999999994</v>
+        <v>-89.45</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>6</v>
@@ -1239,13 +1263,13 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38" s="2">
-        <v>141.55000000000001</v>
+        <v>148.25</v>
       </c>
       <c r="C38" s="2">
-        <v>-93.9375</v>
+        <v>-89.737499999999997</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>6</v>
@@ -1256,13 +1280,13 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B39" s="2">
-        <v>141.5</v>
+        <v>148.19999999999999</v>
       </c>
       <c r="C39" s="2">
-        <v>-87.9375</v>
+        <v>-83.8</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>6</v>
@@ -1273,13 +1297,13 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B40" s="2">
-        <v>144.55000000000001</v>
+        <v>151.19999999999999</v>
       </c>
       <c r="C40" s="2">
-        <v>-117.15</v>
+        <v>-113</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>6</v>
@@ -1290,13 +1314,13 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B41" s="2">
-        <v>138.6</v>
+        <v>145.30000000000001</v>
       </c>
       <c r="C41" s="2">
-        <v>-116.9</v>
+        <v>-112.7</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>6</v>
@@ -1307,13 +1331,13 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B42" s="2">
-        <v>151</v>
+        <v>157.69999999999999</v>
       </c>
       <c r="C42" s="2">
-        <v>-117.5</v>
+        <v>-113.3</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>6</v>
@@ -1324,13 +1348,13 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="2" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="B43" s="2">
-        <v>153.6</v>
+        <v>133.1</v>
       </c>
       <c r="C43" s="2">
-        <v>-88.037499999999994</v>
+        <v>-113.3</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>6</v>
@@ -1341,13 +1365,13 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="2" t="s">
-        <v>46</v>
+        <v>78</v>
       </c>
       <c r="B44" s="2">
-        <v>135.1</v>
+        <v>131.2475</v>
       </c>
       <c r="C44" s="2">
-        <v>-86.337500000000006</v>
+        <v>-112.3</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>6</v>
@@ -1358,47 +1382,47 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="2" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="B45" s="2">
-        <v>144</v>
+        <v>133.1</v>
       </c>
       <c r="C45" s="2">
-        <v>-87.137500000000003</v>
+        <v>-112.3</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E45" s="2">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="2" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="B46" s="2">
-        <v>143.9</v>
+        <v>157.30000000000001</v>
       </c>
       <c r="C46" s="2">
-        <v>-114.6</v>
+        <v>-82.2</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E46" s="2">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B47" s="2">
-        <v>156.1</v>
+        <v>138.75</v>
       </c>
       <c r="C47" s="2">
-        <v>-99.287499999999994</v>
+        <v>-82</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>6</v>
@@ -1409,47 +1433,47 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B48" s="2">
-        <v>156.1</v>
+        <v>148.19999999999999</v>
       </c>
       <c r="C48" s="2">
-        <v>-100.78749999999999</v>
+        <v>-82.1</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E48" s="2">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="2" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="B49" s="2">
-        <v>156.1</v>
+        <v>150.6</v>
       </c>
       <c r="C49" s="2">
-        <v>-102.28749999999999</v>
+        <v>-110.4</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E49" s="2">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B50" s="2">
-        <v>156.1</v>
+        <v>160.05000000000001</v>
       </c>
       <c r="C50" s="2">
-        <v>-103.78749999999999</v>
+        <v>-94.85</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>6</v>
@@ -1460,13 +1484,13 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B51" s="2">
-        <v>156.1</v>
+        <v>160.0625</v>
       </c>
       <c r="C51" s="2">
-        <v>-105.28749999999999</v>
+        <v>-96.8</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>6</v>
@@ -1477,115 +1501,115 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B52" s="2">
-        <v>160.63749999999999</v>
+        <v>160.05000000000001</v>
       </c>
       <c r="C52" s="2">
-        <v>-103.8</v>
+        <v>-97.9</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E52" s="2">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B53" s="2">
-        <v>162.30000000000001</v>
+        <v>160.05000000000001</v>
       </c>
       <c r="C53" s="2">
-        <v>-116.4375</v>
+        <v>-99.8</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E53" s="2">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B54" s="2">
-        <v>144.1</v>
+        <v>160.05000000000001</v>
       </c>
       <c r="C54" s="2">
-        <v>-92.9375</v>
+        <v>-100.9</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E54" s="2">
-        <v>-90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B55" s="2">
-        <v>145.30000000000001</v>
+        <v>165.6</v>
       </c>
       <c r="C55" s="2">
-        <v>-108.53749999999999</v>
+        <v>-99.6</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E55" s="2">
-        <v>90</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="2" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="B56" s="2">
-        <v>143.30000000000001</v>
+        <v>163.6</v>
       </c>
       <c r="C56" s="2">
-        <v>-108.3</v>
+        <v>-110.5</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E56" s="2">
-        <v>0</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="2" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="B57" s="2">
-        <v>141.4</v>
+        <v>136.4</v>
       </c>
       <c r="C57" s="2">
-        <v>-108.3</v>
+        <v>-115.4</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E57" s="2">
-        <v>180</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="2" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="B58" s="2">
-        <v>137.15</v>
+        <v>142.19999999999999</v>
       </c>
       <c r="C58" s="2">
-        <v>-118.78749999999999</v>
+        <v>-115.4</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>6</v>
@@ -1596,13 +1620,13 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="2" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="B59" s="2">
-        <v>134.4</v>
+        <v>144.05000000000001</v>
       </c>
       <c r="C59" s="2">
-        <v>-118.78749999999999</v>
+        <v>-83.91</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>6</v>
@@ -1613,115 +1637,115 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="2" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="B60" s="2">
-        <v>138.4</v>
+        <v>163</v>
       </c>
       <c r="C60" s="2">
-        <v>-91.65</v>
+        <v>-88.9</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E60" s="2">
-        <v>0</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B61" s="2">
-        <v>138.4</v>
+        <v>150.69999999999999</v>
       </c>
       <c r="C61" s="2">
-        <v>-90.55</v>
+        <v>-89</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E61" s="2">
-        <v>180</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B62" s="2">
-        <v>148.1</v>
+        <v>152.1</v>
       </c>
       <c r="C62" s="2">
-        <v>-97.8</v>
+        <v>-104.2</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E62" s="2">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="2" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B63" s="2">
-        <v>135.9</v>
+        <v>150.1</v>
       </c>
       <c r="C63" s="2">
-        <v>-88.4</v>
+        <v>-104.1</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E63" s="2">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="2" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="B64" s="2">
-        <v>150.5</v>
+        <v>148.1</v>
       </c>
       <c r="C64" s="2">
-        <v>-91.037499999999994</v>
+        <v>-104.1</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E64" s="2">
-        <v>-90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B65" s="2">
-        <v>131.9</v>
+        <v>141.69999999999999</v>
       </c>
       <c r="C65" s="2">
-        <v>-89.537499999999994</v>
+        <v>-112.7</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E65" s="2">
-        <v>-90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B66" s="2">
-        <v>145.80000000000001</v>
+        <v>136.9</v>
       </c>
       <c r="C66" s="2">
-        <v>-113</v>
+        <v>-112.7</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>6</v>
@@ -1732,70 +1756,206 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B67" s="2">
-        <v>150.65</v>
+        <v>145.1</v>
       </c>
       <c r="C67" s="2">
-        <v>-97.037499999999994</v>
+        <v>-87.45</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E67" s="2">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B68" s="2">
-        <v>141.30000000000001</v>
+        <v>145.1</v>
       </c>
       <c r="C68" s="2">
-        <v>-90.9375</v>
+        <v>-86.3</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E68" s="2">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="2" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="B69" s="2">
-        <v>141.65</v>
+        <v>154.25</v>
       </c>
       <c r="C69" s="2">
-        <v>-117.05</v>
+        <v>-93.6</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E69" s="2">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B70" s="2">
-        <v>152.24</v>
+        <v>142</v>
       </c>
       <c r="C70" s="2">
-        <v>-120.36</v>
+        <v>-84.3</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E70" s="2">
         <v>90</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B71" s="2">
+        <v>157.19999999999999</v>
+      </c>
+      <c r="C71" s="2">
+        <v>-86.85</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E71" s="2">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B72" s="2">
+        <v>138.6</v>
+      </c>
+      <c r="C72" s="2">
+        <v>-86.85</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E72" s="2">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>63</v>
+      </c>
+      <c r="B73">
+        <v>152.5</v>
+      </c>
+      <c r="C73">
+        <v>-108.95</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>64</v>
+      </c>
+      <c r="B74">
+        <v>155.69999999999999</v>
+      </c>
+      <c r="C74">
+        <v>-91.45</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E74">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>65</v>
+      </c>
+      <c r="B75">
+        <v>148</v>
+      </c>
+      <c r="C75">
+        <v>-86.85</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E75">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>71</v>
+      </c>
+      <c r="B76">
+        <v>148.30000000000001</v>
+      </c>
+      <c r="C76">
+        <v>-112.9</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E76">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>72</v>
+      </c>
+      <c r="B77">
+        <v>159</v>
+      </c>
+      <c r="C77">
+        <v>-116.2</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E77">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>82</v>
+      </c>
+      <c r="B78">
+        <v>132.41249999999999</v>
+      </c>
+      <c r="C78">
+        <v>-110.2</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>